<commit_message>
Add invalid phones test
</commit_message>
<xml_diff>
--- a/server/src/test/resources/phones.xlsx
+++ b/server/src/test/resources/phones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ithersta/unistart-bot/server/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9015FB-64C1-244B-B713-BD023FDD5AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44D20C0-F017-FD40-9ABD-96D471D9A499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="720" windowWidth="36800" windowHeight="20640" xr2:uid="{EFB8216A-2C36-FC4C-A2D0-52C57292A8EB}"/>
+    <workbookView xWindow="1360" yWindow="11100" windowWidth="12320" windowHeight="10260" xr2:uid="{EFB8216A-2C36-FC4C-A2D0-52C57292A8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>